<commit_message>
[NEW FEATURE] support to set the specified color of word
</commit_message>
<xml_diff>
--- a/wordcloud/data.xlsx
+++ b/wordcloud/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7695"/>
+    <workbookView windowWidth="25600" windowHeight="12200"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>name</t>
+    <t>word</t>
   </si>
   <si>
-    <t>value</t>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>color</t>
   </si>
   <si>
     <t>关键词1</t>
   </si>
   <si>
+    <t>#CCFFE5</t>
+  </si>
+  <si>
     <t>关键词2</t>
   </si>
   <si>
+    <t>#9999FF</t>
+  </si>
+  <si>
     <t>关键词3</t>
+  </si>
+  <si>
+    <t>#000000</t>
   </si>
   <si>
     <t>关键词4</t>
@@ -1203,52 +1215,64 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.81666666666667" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="2" max="2" width="12.1272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1256,7 +1280,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1264,7 +1288,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1</v>

</xml_diff>